<commit_message>
Changed some previous off days.
</commit_message>
<xml_diff>
--- a/2016-ElregVacation.xlsx
+++ b/2016-ElregVacation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elreg_Emir\Desktop\ElregDocuments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elreg\ElregDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8550" tabRatio="328" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8550" tabRatio="328" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Ernad" sheetId="80" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="58">
   <si>
     <t>April</t>
   </si>
@@ -166,18 +166,6 @@
     <t>Slobodni dani</t>
   </si>
   <si>
-    <t>11. maj, 6. juni</t>
-  </si>
-  <si>
-    <t>4. - 8. juni</t>
-  </si>
-  <si>
-    <t>15. - 19. august</t>
-  </si>
-  <si>
-    <t>22. - 26. august</t>
-  </si>
-  <si>
     <t>broj dana</t>
   </si>
   <si>
@@ -205,7 +193,19 @@
     <t>14. septembar - 16. septembar</t>
   </si>
   <si>
-    <t>19. septembar - 30. septembar</t>
+    <t>19. decembar - 30. decembar</t>
+  </si>
+  <si>
+    <t>04.07 - 8.07.</t>
+  </si>
+  <si>
+    <t>15.08. - 19. 08</t>
+  </si>
+  <si>
+    <t>22.08. - 26.08</t>
+  </si>
+  <si>
+    <t>29. 02., 11.05.,  06.06.</t>
   </si>
 </sst>
 </file>
@@ -1026,15 +1026,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="7" borderId="1" xfId="35" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1046,6 +1037,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="11" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2020,44 +2020,44 @@
       <c r="AD1" s="4"/>
     </row>
     <row r="2" spans="1:33" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="66"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="71"/>
       <c r="H2" s="21"/>
-      <c r="I2" s="64" t="s">
+      <c r="I2" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="66"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="71"/>
       <c r="P2" s="21"/>
-      <c r="Q2" s="64" t="s">
+      <c r="Q2" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="66"/>
-      <c r="Y2" s="64" t="s">
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="70"/>
+      <c r="V2" s="70"/>
+      <c r="W2" s="71"/>
+      <c r="Y2" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="65"/>
-      <c r="AE2" s="66"/>
+      <c r="Z2" s="70"/>
+      <c r="AA2" s="70"/>
+      <c r="AB2" s="70"/>
+      <c r="AC2" s="70"/>
+      <c r="AD2" s="70"/>
+      <c r="AE2" s="71"/>
     </row>
     <row r="3" spans="1:33" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
@@ -2639,45 +2639,45 @@
       <c r="AE10" s="7"/>
     </row>
     <row r="11" spans="1:33" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="66"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="71"/>
       <c r="H11" s="21"/>
-      <c r="I11" s="64" t="s">
+      <c r="I11" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="65"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="65"/>
-      <c r="N11" s="65"/>
-      <c r="O11" s="66"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="70"/>
+      <c r="L11" s="70"/>
+      <c r="M11" s="70"/>
+      <c r="N11" s="70"/>
+      <c r="O11" s="71"/>
       <c r="P11" s="21"/>
-      <c r="Q11" s="64" t="s">
+      <c r="Q11" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="R11" s="65"/>
-      <c r="S11" s="65"/>
-      <c r="T11" s="65"/>
-      <c r="U11" s="65"/>
-      <c r="V11" s="65"/>
-      <c r="W11" s="66"/>
+      <c r="R11" s="70"/>
+      <c r="S11" s="70"/>
+      <c r="T11" s="70"/>
+      <c r="U11" s="70"/>
+      <c r="V11" s="70"/>
+      <c r="W11" s="71"/>
       <c r="X11" s="21"/>
-      <c r="Y11" s="64" t="s">
+      <c r="Y11" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="Z11" s="65"/>
-      <c r="AA11" s="65"/>
-      <c r="AB11" s="65"/>
-      <c r="AC11" s="65"/>
-      <c r="AD11" s="65"/>
-      <c r="AE11" s="66"/>
+      <c r="Z11" s="70"/>
+      <c r="AA11" s="70"/>
+      <c r="AB11" s="70"/>
+      <c r="AC11" s="70"/>
+      <c r="AD11" s="70"/>
+      <c r="AE11" s="71"/>
     </row>
     <row r="12" spans="1:33" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
@@ -3290,44 +3290,44 @@
       <c r="W19" s="9"/>
     </row>
     <row r="20" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="64" t="s">
+      <c r="A20" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="66"/>
-      <c r="I20" s="64" t="s">
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="71"/>
+      <c r="I20" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="J20" s="65"/>
-      <c r="K20" s="65"/>
-      <c r="L20" s="65"/>
-      <c r="M20" s="65"/>
-      <c r="N20" s="65"/>
-      <c r="O20" s="66"/>
+      <c r="J20" s="70"/>
+      <c r="K20" s="70"/>
+      <c r="L20" s="70"/>
+      <c r="M20" s="70"/>
+      <c r="N20" s="70"/>
+      <c r="O20" s="71"/>
       <c r="P20" s="21"/>
-      <c r="Q20" s="64" t="s">
+      <c r="Q20" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="R20" s="65"/>
-      <c r="S20" s="65"/>
-      <c r="T20" s="65"/>
-      <c r="U20" s="65"/>
-      <c r="V20" s="65"/>
-      <c r="W20" s="66"/>
+      <c r="R20" s="70"/>
+      <c r="S20" s="70"/>
+      <c r="T20" s="70"/>
+      <c r="U20" s="70"/>
+      <c r="V20" s="70"/>
+      <c r="W20" s="71"/>
       <c r="X20" s="21"/>
-      <c r="Y20" s="64" t="s">
+      <c r="Y20" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="Z20" s="65"/>
-      <c r="AA20" s="65"/>
-      <c r="AB20" s="65"/>
-      <c r="AC20" s="65"/>
-      <c r="AD20" s="65"/>
-      <c r="AE20" s="66"/>
+      <c r="Z20" s="70"/>
+      <c r="AA20" s="70"/>
+      <c r="AB20" s="70"/>
+      <c r="AC20" s="70"/>
+      <c r="AD20" s="70"/>
+      <c r="AE20" s="71"/>
     </row>
     <row r="21" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="24" t="s">
@@ -4012,8 +4012,8 @@
   </sheetPr>
   <dimension ref="A1:AJ34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AM21" sqref="AM21"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4052,44 +4052,44 @@
       <c r="AD1" s="4"/>
     </row>
     <row r="2" spans="1:36" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="66"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="71"/>
       <c r="H2" s="21"/>
-      <c r="I2" s="64" t="s">
+      <c r="I2" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="66"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="71"/>
       <c r="P2" s="21"/>
-      <c r="Q2" s="64" t="s">
+      <c r="Q2" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="66"/>
-      <c r="Y2" s="64" t="s">
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="70"/>
+      <c r="V2" s="70"/>
+      <c r="W2" s="71"/>
+      <c r="Y2" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="65"/>
-      <c r="AE2" s="66"/>
+      <c r="Z2" s="70"/>
+      <c r="AA2" s="70"/>
+      <c r="AB2" s="70"/>
+      <c r="AC2" s="70"/>
+      <c r="AD2" s="70"/>
+      <c r="AE2" s="71"/>
     </row>
     <row r="3" spans="1:36" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
@@ -4671,45 +4671,45 @@
       <c r="AE10" s="7"/>
     </row>
     <row r="11" spans="1:36" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="66"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="71"/>
       <c r="H11" s="21"/>
-      <c r="I11" s="64" t="s">
+      <c r="I11" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="65"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="65"/>
-      <c r="N11" s="65"/>
-      <c r="O11" s="66"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="70"/>
+      <c r="L11" s="70"/>
+      <c r="M11" s="70"/>
+      <c r="N11" s="70"/>
+      <c r="O11" s="71"/>
       <c r="P11" s="21"/>
-      <c r="Q11" s="64" t="s">
+      <c r="Q11" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="R11" s="65"/>
-      <c r="S11" s="65"/>
-      <c r="T11" s="65"/>
-      <c r="U11" s="65"/>
-      <c r="V11" s="65"/>
-      <c r="W11" s="66"/>
+      <c r="R11" s="70"/>
+      <c r="S11" s="70"/>
+      <c r="T11" s="70"/>
+      <c r="U11" s="70"/>
+      <c r="V11" s="70"/>
+      <c r="W11" s="71"/>
       <c r="X11" s="21"/>
-      <c r="Y11" s="64" t="s">
+      <c r="Y11" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="Z11" s="65"/>
-      <c r="AA11" s="65"/>
-      <c r="AB11" s="65"/>
-      <c r="AC11" s="65"/>
-      <c r="AD11" s="65"/>
-      <c r="AE11" s="66"/>
+      <c r="Z11" s="70"/>
+      <c r="AA11" s="70"/>
+      <c r="AB11" s="70"/>
+      <c r="AC11" s="70"/>
+      <c r="AD11" s="70"/>
+      <c r="AE11" s="71"/>
       <c r="AJ11" s="22" t="s">
         <v>42</v>
       </c>
@@ -4803,7 +4803,7 @@
         <v>6</v>
       </c>
       <c r="AH12" s="47"/>
-      <c r="AI12" s="69"/>
+      <c r="AI12" s="66"/>
     </row>
     <row r="13" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="32">
@@ -4869,19 +4869,19 @@
       </c>
       <c r="X13" s="16"/>
       <c r="Y13" s="32"/>
-      <c r="Z13" s="68">
+      <c r="Z13" s="65">
         <v>1</v>
       </c>
-      <c r="AA13" s="68">
+      <c r="AA13" s="65">
         <v>2</v>
       </c>
-      <c r="AB13" s="68">
+      <c r="AB13" s="65">
         <v>3</v>
       </c>
-      <c r="AC13" s="68">
-        <v>4</v>
-      </c>
-      <c r="AD13" s="68">
+      <c r="AC13" s="65">
+        <v>4</v>
+      </c>
+      <c r="AD13" s="65">
         <v>5</v>
       </c>
       <c r="AE13" s="34">
@@ -4891,7 +4891,7 @@
       <c r="AH13" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="AI13" s="71">
+      <c r="AI13" s="68">
         <v>42429</v>
       </c>
       <c r="AJ13" s="22">
@@ -4989,7 +4989,7 @@
       <c r="AG14" s="22"/>
       <c r="AH14" s="47"/>
       <c r="AI14" s="50" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="AJ14" s="20">
         <v>10</v>
@@ -5086,7 +5086,7 @@
       <c r="AG15" s="22"/>
       <c r="AH15" s="22"/>
       <c r="AI15" s="50" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="AJ15" s="20">
         <v>3</v>
@@ -5182,7 +5182,7 @@
       </c>
       <c r="AH16" s="22"/>
       <c r="AI16" s="50" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AJ16" s="20">
         <v>10</v>
@@ -5356,44 +5356,44 @@
       <c r="W19" s="9"/>
     </row>
     <row r="20" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="64" t="s">
+      <c r="A20" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="66"/>
-      <c r="I20" s="64" t="s">
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="71"/>
+      <c r="I20" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="J20" s="65"/>
-      <c r="K20" s="65"/>
-      <c r="L20" s="65"/>
-      <c r="M20" s="65"/>
-      <c r="N20" s="65"/>
-      <c r="O20" s="66"/>
+      <c r="J20" s="70"/>
+      <c r="K20" s="70"/>
+      <c r="L20" s="70"/>
+      <c r="M20" s="70"/>
+      <c r="N20" s="70"/>
+      <c r="O20" s="71"/>
       <c r="P20" s="21"/>
-      <c r="Q20" s="64" t="s">
+      <c r="Q20" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="R20" s="65"/>
-      <c r="S20" s="65"/>
-      <c r="T20" s="65"/>
-      <c r="U20" s="65"/>
-      <c r="V20" s="65"/>
-      <c r="W20" s="66"/>
+      <c r="R20" s="70"/>
+      <c r="S20" s="70"/>
+      <c r="T20" s="70"/>
+      <c r="U20" s="70"/>
+      <c r="V20" s="70"/>
+      <c r="W20" s="71"/>
       <c r="X20" s="21"/>
-      <c r="Y20" s="64" t="s">
+      <c r="Y20" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="Z20" s="65"/>
-      <c r="AA20" s="65"/>
-      <c r="AB20" s="65"/>
-      <c r="AC20" s="65"/>
-      <c r="AD20" s="65"/>
-      <c r="AE20" s="66"/>
+      <c r="Z20" s="70"/>
+      <c r="AA20" s="70"/>
+      <c r="AB20" s="70"/>
+      <c r="AC20" s="70"/>
+      <c r="AD20" s="70"/>
+      <c r="AE20" s="71"/>
     </row>
     <row r="21" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="24" t="s">
@@ -5658,10 +5658,10 @@
       <c r="A24" s="33">
         <v>11</v>
       </c>
-      <c r="B24" s="67">
+      <c r="B24" s="64">
         <v>12</v>
       </c>
-      <c r="C24" s="67">
+      <c r="C24" s="64">
         <v>13</v>
       </c>
       <c r="D24" s="55">
@@ -5803,7 +5803,7 @@
       <c r="U25" s="26">
         <v>24</v>
       </c>
-      <c r="V25" s="67">
+      <c r="V25" s="64">
         <v>25</v>
       </c>
       <c r="W25" s="35">
@@ -5902,7 +5902,7 @@
       <c r="Y26" s="33">
         <v>25</v>
       </c>
-      <c r="Z26" s="70">
+      <c r="Z26" s="67">
         <v>26</v>
       </c>
       <c r="AA26" s="55">
@@ -6046,18 +6046,18 @@
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="22" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="22" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -6135,44 +6135,44 @@
       <c r="AD1" s="4"/>
     </row>
     <row r="2" spans="1:35" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="66"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="71"/>
       <c r="H2" s="21"/>
-      <c r="I2" s="64" t="s">
+      <c r="I2" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="66"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="71"/>
       <c r="P2" s="21"/>
-      <c r="Q2" s="64" t="s">
+      <c r="Q2" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="66"/>
-      <c r="Y2" s="64" t="s">
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="70"/>
+      <c r="V2" s="70"/>
+      <c r="W2" s="71"/>
+      <c r="Y2" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="65"/>
-      <c r="AE2" s="66"/>
+      <c r="Z2" s="70"/>
+      <c r="AA2" s="70"/>
+      <c r="AB2" s="70"/>
+      <c r="AC2" s="70"/>
+      <c r="AD2" s="70"/>
+      <c r="AE2" s="71"/>
     </row>
     <row r="3" spans="1:35" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
@@ -6757,45 +6757,45 @@
       </c>
     </row>
     <row r="11" spans="1:35" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="66"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="71"/>
       <c r="H11" s="21"/>
-      <c r="I11" s="64" t="s">
+      <c r="I11" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="65"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="65"/>
-      <c r="N11" s="65"/>
-      <c r="O11" s="66"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="70"/>
+      <c r="L11" s="70"/>
+      <c r="M11" s="70"/>
+      <c r="N11" s="70"/>
+      <c r="O11" s="71"/>
       <c r="P11" s="21"/>
-      <c r="Q11" s="64" t="s">
+      <c r="Q11" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="R11" s="65"/>
-      <c r="S11" s="65"/>
-      <c r="T11" s="65"/>
-      <c r="U11" s="65"/>
-      <c r="V11" s="65"/>
-      <c r="W11" s="66"/>
+      <c r="R11" s="70"/>
+      <c r="S11" s="70"/>
+      <c r="T11" s="70"/>
+      <c r="U11" s="70"/>
+      <c r="V11" s="70"/>
+      <c r="W11" s="71"/>
       <c r="X11" s="21"/>
-      <c r="Y11" s="64" t="s">
+      <c r="Y11" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="Z11" s="65"/>
-      <c r="AA11" s="65"/>
-      <c r="AB11" s="65"/>
-      <c r="AC11" s="65"/>
-      <c r="AD11" s="65"/>
-      <c r="AE11" s="66"/>
+      <c r="Z11" s="70"/>
+      <c r="AA11" s="70"/>
+      <c r="AB11" s="70"/>
+      <c r="AC11" s="70"/>
+      <c r="AD11" s="70"/>
+      <c r="AE11" s="71"/>
       <c r="AG11" s="47" t="s">
         <v>38</v>
       </c>
@@ -7433,44 +7433,44 @@
       <c r="W19" s="9"/>
     </row>
     <row r="20" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="64" t="s">
+      <c r="A20" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="66"/>
-      <c r="I20" s="64" t="s">
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="71"/>
+      <c r="I20" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="J20" s="65"/>
-      <c r="K20" s="65"/>
-      <c r="L20" s="65"/>
-      <c r="M20" s="65"/>
-      <c r="N20" s="65"/>
-      <c r="O20" s="66"/>
+      <c r="J20" s="70"/>
+      <c r="K20" s="70"/>
+      <c r="L20" s="70"/>
+      <c r="M20" s="70"/>
+      <c r="N20" s="70"/>
+      <c r="O20" s="71"/>
       <c r="P20" s="21"/>
-      <c r="Q20" s="64" t="s">
+      <c r="Q20" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="R20" s="65"/>
-      <c r="S20" s="65"/>
-      <c r="T20" s="65"/>
-      <c r="U20" s="65"/>
-      <c r="V20" s="65"/>
-      <c r="W20" s="66"/>
+      <c r="R20" s="70"/>
+      <c r="S20" s="70"/>
+      <c r="T20" s="70"/>
+      <c r="U20" s="70"/>
+      <c r="V20" s="70"/>
+      <c r="W20" s="71"/>
       <c r="X20" s="21"/>
-      <c r="Y20" s="64" t="s">
+      <c r="Y20" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="Z20" s="65"/>
-      <c r="AA20" s="65"/>
-      <c r="AB20" s="65"/>
-      <c r="AC20" s="65"/>
-      <c r="AD20" s="65"/>
-      <c r="AE20" s="66"/>
+      <c r="Z20" s="70"/>
+      <c r="AA20" s="70"/>
+      <c r="AB20" s="70"/>
+      <c r="AC20" s="70"/>
+      <c r="AD20" s="70"/>
+      <c r="AE20" s="71"/>
     </row>
     <row r="21" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="24" t="s">
@@ -8204,44 +8204,44 @@
       <c r="AD1" s="4"/>
     </row>
     <row r="2" spans="1:33" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="66"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="71"/>
       <c r="H2" s="21"/>
-      <c r="I2" s="64" t="s">
+      <c r="I2" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="66"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="71"/>
       <c r="P2" s="21"/>
-      <c r="Q2" s="64" t="s">
+      <c r="Q2" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="66"/>
-      <c r="Y2" s="64" t="s">
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="70"/>
+      <c r="V2" s="70"/>
+      <c r="W2" s="71"/>
+      <c r="Y2" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="65"/>
-      <c r="AE2" s="66"/>
+      <c r="Z2" s="70"/>
+      <c r="AA2" s="70"/>
+      <c r="AB2" s="70"/>
+      <c r="AC2" s="70"/>
+      <c r="AD2" s="70"/>
+      <c r="AE2" s="71"/>
     </row>
     <row r="3" spans="1:33" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
@@ -8823,45 +8823,45 @@
       <c r="AE10" s="7"/>
     </row>
     <row r="11" spans="1:33" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="66"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="71"/>
       <c r="H11" s="21"/>
-      <c r="I11" s="64" t="s">
+      <c r="I11" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="65"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="65"/>
-      <c r="N11" s="65"/>
-      <c r="O11" s="66"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="70"/>
+      <c r="L11" s="70"/>
+      <c r="M11" s="70"/>
+      <c r="N11" s="70"/>
+      <c r="O11" s="71"/>
       <c r="P11" s="21"/>
-      <c r="Q11" s="64" t="s">
+      <c r="Q11" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="R11" s="65"/>
-      <c r="S11" s="65"/>
-      <c r="T11" s="65"/>
-      <c r="U11" s="65"/>
-      <c r="V11" s="65"/>
-      <c r="W11" s="66"/>
+      <c r="R11" s="70"/>
+      <c r="S11" s="70"/>
+      <c r="T11" s="70"/>
+      <c r="U11" s="70"/>
+      <c r="V11" s="70"/>
+      <c r="W11" s="71"/>
       <c r="X11" s="21"/>
-      <c r="Y11" s="64" t="s">
+      <c r="Y11" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="Z11" s="65"/>
-      <c r="AA11" s="65"/>
-      <c r="AB11" s="65"/>
-      <c r="AC11" s="65"/>
-      <c r="AD11" s="65"/>
-      <c r="AE11" s="66"/>
+      <c r="Z11" s="70"/>
+      <c r="AA11" s="70"/>
+      <c r="AB11" s="70"/>
+      <c r="AC11" s="70"/>
+      <c r="AD11" s="70"/>
+      <c r="AE11" s="71"/>
     </row>
     <row r="12" spans="1:33" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
@@ -9465,44 +9465,44 @@
       <c r="W19" s="9"/>
     </row>
     <row r="20" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="64" t="s">
+      <c r="A20" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="66"/>
-      <c r="I20" s="64" t="s">
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="71"/>
+      <c r="I20" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="J20" s="65"/>
-      <c r="K20" s="65"/>
-      <c r="L20" s="65"/>
-      <c r="M20" s="65"/>
-      <c r="N20" s="65"/>
-      <c r="O20" s="66"/>
+      <c r="J20" s="70"/>
+      <c r="K20" s="70"/>
+      <c r="L20" s="70"/>
+      <c r="M20" s="70"/>
+      <c r="N20" s="70"/>
+      <c r="O20" s="71"/>
       <c r="P20" s="21"/>
-      <c r="Q20" s="64" t="s">
+      <c r="Q20" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="R20" s="65"/>
-      <c r="S20" s="65"/>
-      <c r="T20" s="65"/>
-      <c r="U20" s="65"/>
-      <c r="V20" s="65"/>
-      <c r="W20" s="66"/>
+      <c r="R20" s="70"/>
+      <c r="S20" s="70"/>
+      <c r="T20" s="70"/>
+      <c r="U20" s="70"/>
+      <c r="V20" s="70"/>
+      <c r="W20" s="71"/>
       <c r="X20" s="21"/>
-      <c r="Y20" s="64" t="s">
+      <c r="Y20" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="Z20" s="65"/>
-      <c r="AA20" s="65"/>
-      <c r="AB20" s="65"/>
-      <c r="AC20" s="65"/>
-      <c r="AD20" s="65"/>
-      <c r="AE20" s="66"/>
+      <c r="Z20" s="70"/>
+      <c r="AA20" s="70"/>
+      <c r="AB20" s="70"/>
+      <c r="AC20" s="70"/>
+      <c r="AD20" s="70"/>
+      <c r="AE20" s="71"/>
     </row>
     <row r="21" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="24" t="s">
@@ -10185,10 +10185,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AI32"/>
+  <dimension ref="A1:AI34"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH17" sqref="AH17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH18" sqref="AH18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10196,7 +10196,7 @@
     <col min="1" max="31" width="4.28515625" style="20" customWidth="1"/>
     <col min="32" max="32" width="9.140625" style="20"/>
     <col min="33" max="33" width="17.85546875" style="20" customWidth="1"/>
-    <col min="34" max="34" width="19.28515625" style="20" customWidth="1"/>
+    <col min="34" max="34" width="26.42578125" style="20" customWidth="1"/>
     <col min="35" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
@@ -10228,44 +10228,44 @@
       <c r="AD1" s="4"/>
     </row>
     <row r="2" spans="1:35" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="66"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="71"/>
       <c r="H2" s="21"/>
-      <c r="I2" s="64" t="s">
+      <c r="I2" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="66"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="71"/>
       <c r="P2" s="21"/>
-      <c r="Q2" s="64" t="s">
+      <c r="Q2" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="66"/>
-      <c r="Y2" s="64" t="s">
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="70"/>
+      <c r="V2" s="70"/>
+      <c r="W2" s="71"/>
+      <c r="Y2" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="65"/>
-      <c r="AE2" s="66"/>
+      <c r="Z2" s="70"/>
+      <c r="AA2" s="70"/>
+      <c r="AB2" s="70"/>
+      <c r="AC2" s="70"/>
+      <c r="AD2" s="70"/>
+      <c r="AE2" s="71"/>
     </row>
     <row r="3" spans="1:35" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
@@ -10730,7 +10730,7 @@
       <c r="I8" s="33">
         <v>28</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="55">
         <v>29</v>
       </c>
       <c r="K8" s="14"/>
@@ -10846,54 +10846,54 @@
       <c r="AD10" s="7"/>
       <c r="AE10" s="7"/>
       <c r="AI10" s="63" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:35" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="66"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="71"/>
       <c r="H11" s="21"/>
-      <c r="I11" s="64" t="s">
+      <c r="I11" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="65"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="65"/>
-      <c r="N11" s="65"/>
-      <c r="O11" s="66"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="70"/>
+      <c r="L11" s="70"/>
+      <c r="M11" s="70"/>
+      <c r="N11" s="70"/>
+      <c r="O11" s="71"/>
       <c r="P11" s="21"/>
-      <c r="Q11" s="64" t="s">
+      <c r="Q11" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="R11" s="65"/>
-      <c r="S11" s="65"/>
-      <c r="T11" s="65"/>
-      <c r="U11" s="65"/>
-      <c r="V11" s="65"/>
-      <c r="W11" s="66"/>
+      <c r="R11" s="70"/>
+      <c r="S11" s="70"/>
+      <c r="T11" s="70"/>
+      <c r="U11" s="70"/>
+      <c r="V11" s="70"/>
+      <c r="W11" s="71"/>
       <c r="X11" s="21"/>
-      <c r="Y11" s="64" t="s">
+      <c r="Y11" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="Z11" s="65"/>
-      <c r="AA11" s="65"/>
-      <c r="AB11" s="65"/>
-      <c r="AC11" s="65"/>
-      <c r="AD11" s="65"/>
-      <c r="AE11" s="66"/>
+      <c r="Z11" s="70"/>
+      <c r="AA11" s="70"/>
+      <c r="AB11" s="70"/>
+      <c r="AC11" s="70"/>
+      <c r="AD11" s="70"/>
+      <c r="AE11" s="71"/>
       <c r="AG11" s="59" t="s">
         <v>43</v>
       </c>
       <c r="AH11" s="59" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="AI11" s="59">
         <v>2</v>
@@ -10991,10 +10991,10 @@
         <v>36</v>
       </c>
       <c r="AH12" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI12" s="62" t="s">
         <v>45</v>
-      </c>
-      <c r="AI12" s="62" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11083,7 +11083,7 @@
         <v>36</v>
       </c>
       <c r="AH13" s="62" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="AI13" s="62">
         <v>5</v>
@@ -11178,7 +11178,7 @@
         <v>13</v>
       </c>
       <c r="AG14" s="58" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AH14" s="58"/>
       <c r="AI14" s="63"/>
@@ -11275,7 +11275,7 @@
         <v>36</v>
       </c>
       <c r="AH15" s="62" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="AI15" s="62">
         <v>5</v>
@@ -11530,44 +11530,44 @@
       <c r="W19" s="9"/>
     </row>
     <row r="20" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="64" t="s">
+      <c r="A20" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="66"/>
-      <c r="I20" s="64" t="s">
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="71"/>
+      <c r="I20" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="J20" s="65"/>
-      <c r="K20" s="65"/>
-      <c r="L20" s="65"/>
-      <c r="M20" s="65"/>
-      <c r="N20" s="65"/>
-      <c r="O20" s="66"/>
+      <c r="J20" s="70"/>
+      <c r="K20" s="70"/>
+      <c r="L20" s="70"/>
+      <c r="M20" s="70"/>
+      <c r="N20" s="70"/>
+      <c r="O20" s="71"/>
       <c r="P20" s="21"/>
-      <c r="Q20" s="64" t="s">
+      <c r="Q20" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="R20" s="65"/>
-      <c r="S20" s="65"/>
-      <c r="T20" s="65"/>
-      <c r="U20" s="65"/>
-      <c r="V20" s="65"/>
-      <c r="W20" s="66"/>
+      <c r="R20" s="70"/>
+      <c r="S20" s="70"/>
+      <c r="T20" s="70"/>
+      <c r="U20" s="70"/>
+      <c r="V20" s="70"/>
+      <c r="W20" s="71"/>
       <c r="X20" s="21"/>
-      <c r="Y20" s="64" t="s">
+      <c r="Y20" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="Z20" s="65"/>
-      <c r="AA20" s="65"/>
-      <c r="AB20" s="65"/>
-      <c r="AC20" s="65"/>
-      <c r="AD20" s="65"/>
-      <c r="AE20" s="66"/>
+      <c r="Z20" s="70"/>
+      <c r="AA20" s="70"/>
+      <c r="AB20" s="70"/>
+      <c r="AC20" s="70"/>
+      <c r="AD20" s="70"/>
+      <c r="AE20" s="71"/>
     </row>
     <row r="21" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="24" t="s">
@@ -11832,10 +11832,10 @@
       <c r="A24" s="33">
         <v>11</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="64">
         <v>12</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="64">
         <v>13</v>
       </c>
       <c r="D24" s="14">
@@ -11977,7 +11977,7 @@
       <c r="U25" s="26">
         <v>24</v>
       </c>
-      <c r="V25" s="14">
+      <c r="V25" s="64">
         <v>25</v>
       </c>
       <c r="W25" s="35">
@@ -12216,6 +12216,22 @@
       </c>
       <c r="E32" s="22" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -12290,44 +12306,44 @@
       <c r="AD1" s="4"/>
     </row>
     <row r="2" spans="1:33" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="66"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="71"/>
       <c r="H2" s="21"/>
-      <c r="I2" s="64" t="s">
+      <c r="I2" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="66"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="71"/>
       <c r="P2" s="21"/>
-      <c r="Q2" s="64" t="s">
+      <c r="Q2" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="66"/>
-      <c r="Y2" s="64" t="s">
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="70"/>
+      <c r="V2" s="70"/>
+      <c r="W2" s="71"/>
+      <c r="Y2" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="65"/>
-      <c r="AE2" s="66"/>
+      <c r="Z2" s="70"/>
+      <c r="AA2" s="70"/>
+      <c r="AB2" s="70"/>
+      <c r="AC2" s="70"/>
+      <c r="AD2" s="70"/>
+      <c r="AE2" s="71"/>
     </row>
     <row r="3" spans="1:33" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
@@ -12909,45 +12925,45 @@
       <c r="AE10" s="7"/>
     </row>
     <row r="11" spans="1:33" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="66"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="71"/>
       <c r="H11" s="21"/>
-      <c r="I11" s="64" t="s">
+      <c r="I11" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="65"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="65"/>
-      <c r="N11" s="65"/>
-      <c r="O11" s="66"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="70"/>
+      <c r="L11" s="70"/>
+      <c r="M11" s="70"/>
+      <c r="N11" s="70"/>
+      <c r="O11" s="71"/>
       <c r="P11" s="21"/>
-      <c r="Q11" s="64" t="s">
+      <c r="Q11" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="R11" s="65"/>
-      <c r="S11" s="65"/>
-      <c r="T11" s="65"/>
-      <c r="U11" s="65"/>
-      <c r="V11" s="65"/>
-      <c r="W11" s="66"/>
+      <c r="R11" s="70"/>
+      <c r="S11" s="70"/>
+      <c r="T11" s="70"/>
+      <c r="U11" s="70"/>
+      <c r="V11" s="70"/>
+      <c r="W11" s="71"/>
       <c r="X11" s="21"/>
-      <c r="Y11" s="64" t="s">
+      <c r="Y11" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="Z11" s="65"/>
-      <c r="AA11" s="65"/>
-      <c r="AB11" s="65"/>
-      <c r="AC11" s="65"/>
-      <c r="AD11" s="65"/>
-      <c r="AE11" s="66"/>
+      <c r="Z11" s="70"/>
+      <c r="AA11" s="70"/>
+      <c r="AB11" s="70"/>
+      <c r="AC11" s="70"/>
+      <c r="AD11" s="70"/>
+      <c r="AE11" s="71"/>
     </row>
     <row r="12" spans="1:33" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
@@ -13551,44 +13567,44 @@
       <c r="W19" s="9"/>
     </row>
     <row r="20" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="64" t="s">
+      <c r="A20" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="66"/>
-      <c r="I20" s="64" t="s">
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="71"/>
+      <c r="I20" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="J20" s="65"/>
-      <c r="K20" s="65"/>
-      <c r="L20" s="65"/>
-      <c r="M20" s="65"/>
-      <c r="N20" s="65"/>
-      <c r="O20" s="66"/>
+      <c r="J20" s="70"/>
+      <c r="K20" s="70"/>
+      <c r="L20" s="70"/>
+      <c r="M20" s="70"/>
+      <c r="N20" s="70"/>
+      <c r="O20" s="71"/>
       <c r="P20" s="21"/>
-      <c r="Q20" s="64" t="s">
+      <c r="Q20" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="R20" s="65"/>
-      <c r="S20" s="65"/>
-      <c r="T20" s="65"/>
-      <c r="U20" s="65"/>
-      <c r="V20" s="65"/>
-      <c r="W20" s="66"/>
+      <c r="R20" s="70"/>
+      <c r="S20" s="70"/>
+      <c r="T20" s="70"/>
+      <c r="U20" s="70"/>
+      <c r="V20" s="70"/>
+      <c r="W20" s="71"/>
       <c r="X20" s="21"/>
-      <c r="Y20" s="64" t="s">
+      <c r="Y20" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="Z20" s="65"/>
-      <c r="AA20" s="65"/>
-      <c r="AB20" s="65"/>
-      <c r="AC20" s="65"/>
-      <c r="AD20" s="65"/>
-      <c r="AE20" s="66"/>
+      <c r="Z20" s="70"/>
+      <c r="AA20" s="70"/>
+      <c r="AB20" s="70"/>
+      <c r="AC20" s="70"/>
+      <c r="AD20" s="70"/>
+      <c r="AE20" s="71"/>
     </row>
     <row r="21" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="24" t="s">

</xml_diff>

<commit_message>
29-ti mart stavljen da svima bude isto (slobodan dan)
</commit_message>
<xml_diff>
--- a/2016-ElregVacation.xlsx
+++ b/2016-ElregVacation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8556" tabRatio="328"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8556" tabRatio="328" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Ernad" sheetId="80" r:id="rId1"/>
@@ -2019,7 +2019,7 @@
   </sheetPr>
   <dimension ref="A1:AG33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
@@ -6134,7 +6134,7 @@
   <dimension ref="A1:AI33"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6676,7 +6676,7 @@
       <c r="I8" s="33">
         <v>28</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="28">
         <v>29</v>
       </c>
       <c r="K8" s="14"/>
@@ -12356,8 +12356,8 @@
   </sheetPr>
   <dimension ref="A1:AG32"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -12896,7 +12896,7 @@
       <c r="I8" s="33">
         <v>28</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="28">
         <v>29</v>
       </c>
       <c r="K8" s="14"/>

</xml_diff>